<commit_message>
Fixes as asked for in pull request
</commit_message>
<xml_diff>
--- a/powerboard_monitoring/Bill of Materials.xlsx
+++ b/powerboard_monitoring/Bill of Materials.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -194,31 +194,16 @@
     <t>C1</t>
   </si>
   <si>
-    <t>CAP TANT 0.1UF 35V 20% 1206</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T491A104M035AT </t>
-  </si>
-  <si>
-    <t>https://content.kemet.com/datasheets/KEM_T2005_T491.pdf</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
-    <t>Column1</t>
+    <t>CAP CER 0.1UF 50V X7R 1206</t>
+  </si>
+  <si>
+    <t>C1206C104K5RAC7867</t>
+  </si>
+  <si>
+    <t>https://content.kemet.com/datasheets/KEM_C1002_X7R_SMD.pdf</t>
   </si>
 </sst>
 </file>
@@ -289,27 +274,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <b val="0"/>
@@ -345,6 +310,46 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -360,7 +365,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11EA9FB5-2EF9-4CF3-8402-3C0B39A99038}" name="Table1" displayName="Table1" ref="A1:H14" totalsRowCount="1" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11EA9FB5-2EF9-4CF3-8402-3C0B39A99038}" name="Table1" displayName="Table1" ref="A1:H14" totalsRowCount="1" headerRowDxfId="3">
   <autoFilter ref="A1:H13" xr:uid="{6B74E4FE-A6EE-4EEA-A3C5-1EF076D27B91}"/>
   <sortState ref="A2:H13">
     <sortCondition ref="A1:A13"/>
@@ -370,10 +375,10 @@
     <tableColumn id="2" xr3:uid="{3111B958-9D19-4CE2-B16D-CB121FC81A8D}" name="Schematic Part Number"/>
     <tableColumn id="3" xr3:uid="{D938A151-9A65-4F4F-8C7A-6AB63B732AE7}" name="Name"/>
     <tableColumn id="4" xr3:uid="{93BB4C26-6775-4C71-8DEC-4711D1F4FE9A}" name="Quantity" totalsRowFunction="sum"/>
-    <tableColumn id="5" xr3:uid="{259FB887-FE2E-4C9E-8D33-242FF04CC8B6}" name="Price" totalsRowFunction="sum" dataDxfId="0" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{259FB887-FE2E-4C9E-8D33-242FF04CC8B6}" name="Price" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="1" dataCellStyle="Currency"/>
     <tableColumn id="6" xr3:uid="{32C04940-8F48-4233-A975-6AC84FAEC610}" name="Manufacturer Code"/>
     <tableColumn id="7" xr3:uid="{1E27B34F-61D1-442B-B0C5-7C2A0E210C5A}" name="Order Status"/>
-    <tableColumn id="8" xr3:uid="{47E4AE3E-C5AE-4D8D-8B44-C3419765BE9E}" name="Link to Datasheet" totalsRowDxfId="1" dataCellStyle="Hyperlink"/>
+    <tableColumn id="8" xr3:uid="{47E4AE3E-C5AE-4D8D-8B44-C3419765BE9E}" name="Link to Datasheet" totalsRowDxfId="0" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -679,7 +684,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -728,7 +733,7 @@
         <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -737,10 +742,10 @@
         <v>0.65</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -998,7 +1003,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D14">
         <f>SUBTOTAL(109,Table1[Quantity])</f>
@@ -1025,11 +1030,12 @@
     <hyperlink ref="H4" r:id="rId8" xr:uid="{E8A85176-1725-418A-BF8A-ACE9AC1FD8F2}"/>
     <hyperlink ref="H5" r:id="rId9" xr:uid="{FB6EA38D-3B62-4BC8-BD5F-5D272ACF0A3F}"/>
     <hyperlink ref="H6" r:id="rId10" xr:uid="{9A2B538B-B0FA-44DF-804C-C844787EAA28}"/>
+    <hyperlink ref="H2" r:id="rId11" xr:uid="{715DE3BF-128A-4A0B-9292-8FA12217C2D8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>